<commit_message>
more efforts to gather capital stocks data
</commit_message>
<xml_diff>
--- a/sids data/Gross Capital - Summary.xlsx
+++ b/sids data/Gross Capital - Summary.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -470,12 +470,12 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="20.54296875" customWidth="1"/>
+    <col min="4" max="4" width="33.6328125" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.26953125" customWidth="1"/>
     <col min="7" max="7" width="17.81640625" customWidth="1"/>

</xml_diff>